<commit_message>
Versão final do planejamento
Enviando versão final 100% preenchida da planilha de gerenciamento.
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/Planejamento e Controle do Projeto.xlsx
+++ b/Gerenciamento de Projeto/Planejamento e Controle do Projeto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\GitHub\Grupo1\Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6069DC8D-E055-496B-98B4-DD0C6EAA58F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F54B7E-CC48-4C03-A43A-4B0EA371BC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="797" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="797" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="10" r:id="rId1"/>
@@ -1904,7 +1904,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="272">
   <si>
     <t>Iniciação</t>
   </si>
@@ -2406,19 +2406,10 @@
     <t>Arquivos/Tabelas</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Endereço</t>
-  </si>
-  <si>
     <t>Funções de Dados (Arquivo/Tabela)</t>
   </si>
   <si>
     <t>Caso de Uso/História</t>
-  </si>
-  <si>
-    <t>Manter Cliente</t>
   </si>
   <si>
     <t>Comunicação de Dados</t>
@@ -2523,9 +2514,6 @@
     <t xml:space="preserve">Esforço estimado (Horas): </t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Utilização de Equipamento</t>
   </si>
   <si>
@@ -2814,6 +2802,9 @@
   </si>
   <si>
     <t>1. Buscar outras fontes de conhecimento 2. Buscar entender melhor o que se é solicitado</t>
+  </si>
+  <si>
+    <t>Usuários</t>
   </si>
 </sst>
 </file>
@@ -3532,7 +3523,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3941,6 +3932,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="29" fillId="9" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4023,53 +4018,59 @@
     <xf numFmtId="0" fontId="28" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4119,17 +4120,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="29" fillId="9" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
@@ -6486,18 +6476,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
+      <c r="A2" s="144" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6515,10 +6505,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C4" s="139" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6526,10 +6516,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C5" s="139" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6537,10 +6527,10 @@
         <v>45</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C6" s="139" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6632,92 +6622,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="155" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="F1" s="147" t="s">
-        <v>214</v>
-      </c>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="148"/>
-      <c r="L1" s="148"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="F1" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="149"/>
     </row>
     <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="149" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="F2" s="151" t="s">
-        <v>242</v>
-      </c>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
+      <c r="A2" s="150" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="F2" s="152" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
     </row>
     <row r="3" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="130" t="s">
         <v>133</v>
       </c>
       <c r="B3" s="130" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C3" s="130" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D3" s="130" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F3" s="130" t="s">
         <v>133</v>
       </c>
       <c r="G3" s="131" t="s">
-        <v>212</v>
-      </c>
-      <c r="H3" s="153" t="s">
-        <v>214</v>
-      </c>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
+        <v>208</v>
+      </c>
+      <c r="H3" s="154" t="s">
+        <v>210</v>
+      </c>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
     </row>
     <row r="4" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="145"/>
-      <c r="C4" s="146"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="147"/>
       <c r="D4" s="123" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="121" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G4" s="121" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="H4" s="123" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J4" s="123" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="K4" s="128" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="L4" s="123" t="s">
         <v>25</v>
@@ -6731,7 +6721,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="114" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D5" s="125">
         <v>5</v>
@@ -6740,7 +6730,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="114" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H5" s="122">
         <v>10</v>
@@ -6767,7 +6757,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="114" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D6" s="125">
         <v>5</v>
@@ -6776,7 +6766,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="114" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H6" s="122">
         <v>5</v>
@@ -6803,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="114" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D7" s="125">
         <v>6</v>
@@ -6812,7 +6802,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="114" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H7" s="122">
         <v>10</v>
@@ -6839,7 +6829,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="114" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D8" s="125">
         <v>6</v>
@@ -6863,7 +6853,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="114" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D9" s="125">
         <v>5</v>
@@ -6887,7 +6877,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="114" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D10" s="125">
         <v>2</v>
@@ -6904,11 +6894,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="146"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="147"/>
       <c r="D11" s="123">
         <f>SUM(D5:D10)</f>
         <v>29</v>
@@ -6932,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D12" s="125">
         <v>1</v>
@@ -6956,7 +6946,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="114" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D13" s="125">
         <v>20</v>
@@ -6980,7 +6970,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D14" s="125">
         <v>6</v>
@@ -7004,7 +6994,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="117" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D15" s="125">
         <v>1</v>
@@ -7028,7 +7018,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="140" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D16" s="125">
         <v>2</v>
@@ -7052,7 +7042,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="140" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D17" s="125">
         <v>5</v>
@@ -7076,7 +7066,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="117" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D18" s="125">
         <v>1</v>
@@ -7100,7 +7090,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="117" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D19" s="125">
         <v>10</v>
@@ -7124,7 +7114,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="117" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D20" s="125">
         <v>5</v>
@@ -7145,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="117" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D21" s="125">
         <v>3</v>
@@ -7159,11 +7149,11 @@
       <c r="L21" s="116"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="144" t="s">
+      <c r="A22" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="123">
         <f>SUM(D12:D21)</f>
         <v>54</v>
@@ -7184,7 +7174,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="114" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D23" s="125">
         <v>2</v>
@@ -7205,7 +7195,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="117" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D24" s="125">
         <v>5</v>
@@ -7219,7 +7209,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="140" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D25" s="125">
         <v>5</v>
@@ -7233,7 +7223,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="140" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D26" s="125">
         <v>10</v>
@@ -7247,7 +7237,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="140" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D27" s="125">
         <v>3</v>
@@ -7261,7 +7251,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="140" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D28" s="125">
         <v>5</v>
@@ -7275,7 +7265,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="117" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D29" s="125">
         <v>5</v>
@@ -7289,7 +7279,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="140" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D30" s="125">
         <v>5</v>
@@ -7303,7 +7293,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="140" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D31" s="125">
         <v>10</v>
@@ -7317,7 +7307,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="140" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D32" s="125">
         <v>3</v>
@@ -7331,7 +7321,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="140" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D33" s="125">
         <v>5</v>
@@ -7345,7 +7335,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="117" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D34" s="125">
         <v>5</v>
@@ -7359,7 +7349,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="140" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D35" s="125">
         <v>5</v>
@@ -7373,7 +7363,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="140" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D36" s="125">
         <v>15</v>
@@ -7387,7 +7377,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="140" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D37" s="125">
         <v>2</v>
@@ -7401,7 +7391,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="140" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D38" s="125">
         <v>3</v>
@@ -7415,7 +7405,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="117" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D39" s="125">
         <v>2</v>
@@ -7429,18 +7419,18 @@
         <v>2</v>
       </c>
       <c r="C40" s="117" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D40" s="125">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="144" t="s">
+      <c r="A41" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="145"/>
-      <c r="C41" s="146"/>
+      <c r="B41" s="146"/>
+      <c r="C41" s="147"/>
       <c r="D41" s="123">
         <f>SUM(D23:D40)</f>
         <v>95</v>
@@ -7454,7 +7444,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="114" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D42" s="125">
         <v>2</v>
@@ -7468,7 +7458,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="117" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D43" s="125">
         <v>2</v>
@@ -7482,7 +7472,7 @@
         <v>3</v>
       </c>
       <c r="C44" s="117" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D44" s="125">
         <v>3</v>
@@ -7496,7 +7486,7 @@
         <v>3</v>
       </c>
       <c r="C45" s="117" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D45" s="125">
         <v>5</v>
@@ -7510,7 +7500,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="114" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D46" s="125">
         <v>2</v>
@@ -7524,7 +7514,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="114" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D47" s="125">
         <v>5</v>
@@ -7538,7 +7528,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="114" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D48" s="125">
         <v>3</v>
@@ -7552,7 +7542,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="114" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D49" s="125">
         <v>2</v>
@@ -7566,16 +7556,16 @@
         <v>3</v>
       </c>
       <c r="C50" s="117" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D50" s="125">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12" x14ac:dyDescent="0.2">
-      <c r="A51" s="144"/>
-      <c r="B51" s="145"/>
-      <c r="C51" s="146"/>
+      <c r="A51" s="145"/>
+      <c r="B51" s="146"/>
+      <c r="C51" s="147"/>
       <c r="D51" s="123">
         <f>SUM(D42:D50)</f>
         <v>26</v>
@@ -7626,23 +7616,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
+      <c r="A1" s="157" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
     </row>
     <row r="2" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B4" s="136">
         <f>'Backlog Produto'!$D$52</f>
@@ -7654,18 +7644,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B5" s="26">
         <v>0.4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B6" s="15">
         <v>3</v>
@@ -7674,7 +7664,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B7" s="15">
         <v>12.5</v>
@@ -7685,7 +7675,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B8" s="134">
         <f>B6*B7*2</f>
@@ -7697,19 +7687,19 @@
     </row>
     <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B9" s="133">
         <f>B11/2</f>
         <v>3.8080000000000003</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B10" s="135">
         <f>B4+(B4*B5)</f>
@@ -7721,7 +7711,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B11" s="134">
         <f>B10/B8*2</f>
@@ -7733,7 +7723,7 @@
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B12" s="133">
         <f>B11/4</f>
@@ -7744,11 +7734,11 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="157" t="s">
+      <c r="A14" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="157"/>
-      <c r="C14" s="157"/>
+      <c r="B14" s="158"/>
+      <c r="C14" s="158"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -7790,7 +7780,7 @@
     </row>
     <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B19" s="137">
         <f>B16+B18</f>
@@ -7819,7 +7809,7 @@
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B22" s="137">
         <f>B19+B21</f>
@@ -7843,8 +7833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7861,43 +7851,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="158" t="s">
-        <v>185</v>
-      </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
+      <c r="A1" s="159" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="162" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="163"/>
+      <c r="B2" s="164"/>
       <c r="C2" s="74" t="e">
         <f>Planejamento!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="161" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="160"/>
+      <c r="E2" s="161"/>
       <c r="F2" s="75" t="e">
         <f>Planejamento!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G2" s="161" t="s">
+      <c r="G2" s="162" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="164"/>
       <c r="K2" s="74">
         <f>Planejamento!$B$10</f>
         <v>285.60000000000002</v>
@@ -7906,17 +7896,17 @@
     <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="76"/>
       <c r="B3" s="77"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="165" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
       <c r="F3" s="78"/>
-      <c r="G3" s="165" t="s">
+      <c r="G3" s="166" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="166"/>
-      <c r="I3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="79"/>
       <c r="K3" s="80"/>
     </row>
@@ -7960,7 +7950,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="84" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C5" s="85">
         <v>45175</v>
@@ -7968,7 +7958,7 @@
       <c r="D5" s="85">
         <v>45182</v>
       </c>
-      <c r="E5" s="200">
+      <c r="E5" s="142">
         <v>10</v>
       </c>
       <c r="F5" s="87" t="s">
@@ -7988,7 +7978,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="89" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
@@ -7996,7 +7986,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="84" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C6" s="85">
         <v>45187</v>
@@ -8004,23 +7994,23 @@
       <c r="D6" s="85">
         <v>45203</v>
       </c>
-      <c r="E6" s="200">
+      <c r="E6" s="142">
         <v>28</v>
       </c>
       <c r="F6" s="87" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G6" s="85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H6" s="85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I6" s="90" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J6" s="91" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="K6" s="89"/>
     </row>
@@ -8029,7 +8019,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="114" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C7" s="85">
         <v>45204</v>
@@ -8037,23 +8027,23 @@
       <c r="D7" s="85">
         <v>45219</v>
       </c>
-      <c r="E7" s="200">
+      <c r="E7" s="142">
         <v>28</v>
       </c>
       <c r="F7" s="87" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G7" s="85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H7" s="85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I7" s="90" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J7" s="91" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="K7" s="89"/>
     </row>
@@ -8062,7 +8052,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="114" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C8" s="85">
         <v>45222</v>
@@ -8070,23 +8060,23 @@
       <c r="D8" s="85">
         <v>45238</v>
       </c>
-      <c r="E8" s="200">
+      <c r="E8" s="142">
         <v>30</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G8" s="85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H8" s="85" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I8" s="90" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J8" s="91" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="K8" s="89"/>
     </row>
@@ -9096,19 +9086,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -9262,10 +9252,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="173" t="s">
+      <c r="D33" s="169" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="174"/>
+      <c r="E33" s="170"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="D34" s="61">
@@ -9317,137 +9307,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" s="53" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="180" t="s">
+      <c r="A41" s="177" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="180"/>
-      <c r="C41" s="180"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="180"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
-      <c r="J41" s="180"/>
-      <c r="K41" s="180"/>
+      <c r="B41" s="177"/>
+      <c r="C41" s="177"/>
+      <c r="D41" s="177"/>
+      <c r="E41" s="177"/>
+      <c r="F41" s="177"/>
+      <c r="G41" s="177"/>
+      <c r="H41" s="177"/>
+      <c r="I41" s="177"/>
+      <c r="J41" s="177"/>
+      <c r="K41" s="177"/>
     </row>
     <row r="42" spans="1:11" s="53" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="181" t="s">
+      <c r="A42" s="178" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="181"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="181"/>
-      <c r="E42" s="181"/>
-      <c r="F42" s="181"/>
-      <c r="G42" s="181"/>
-      <c r="H42" s="181"/>
-      <c r="I42" s="181"/>
-      <c r="J42" s="181"/>
-      <c r="K42" s="181"/>
+      <c r="B42" s="178"/>
+      <c r="C42" s="178"/>
+      <c r="D42" s="178"/>
+      <c r="E42" s="178"/>
+      <c r="F42" s="178"/>
+      <c r="G42" s="178"/>
+      <c r="H42" s="178"/>
+      <c r="I42" s="178"/>
+      <c r="J42" s="178"/>
+      <c r="K42" s="178"/>
     </row>
     <row r="43" spans="1:11" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="182" t="s">
+      <c r="A43" s="179" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="182"/>
-      <c r="C43" s="182"/>
-      <c r="D43" s="182"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="182"/>
-      <c r="H43" s="182"/>
-      <c r="I43" s="182"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
+      <c r="B43" s="179"/>
+      <c r="C43" s="179"/>
+      <c r="D43" s="179"/>
+      <c r="E43" s="179"/>
+      <c r="F43" s="179"/>
+      <c r="G43" s="179"/>
+      <c r="H43" s="179"/>
+      <c r="I43" s="179"/>
+      <c r="J43" s="179"/>
+      <c r="K43" s="179"/>
     </row>
     <row r="44" spans="1:11" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="183" t="s">
+      <c r="A44" s="180" t="s">
         <v>119</v>
       </c>
-      <c r="B44" s="183"/>
-      <c r="C44" s="183"/>
-      <c r="D44" s="183"/>
-      <c r="E44" s="183"/>
-      <c r="F44" s="183"/>
-      <c r="G44" s="183"/>
-      <c r="H44" s="183"/>
-      <c r="I44" s="183"/>
-      <c r="J44" s="183"/>
-      <c r="K44" s="183"/>
+      <c r="B44" s="180"/>
+      <c r="C44" s="180"/>
+      <c r="D44" s="180"/>
+      <c r="E44" s="180"/>
+      <c r="F44" s="180"/>
+      <c r="G44" s="180"/>
+      <c r="H44" s="180"/>
+      <c r="I44" s="180"/>
+      <c r="J44" s="180"/>
+      <c r="K44" s="180"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="175" t="s">
+      <c r="A46" s="171" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="176"/>
-      <c r="C46" s="176"/>
-      <c r="D46" s="176"/>
-      <c r="E46" s="176"/>
-      <c r="F46" s="176"/>
-      <c r="G46" s="176"/>
-      <c r="H46" s="176"/>
-      <c r="I46" s="176"/>
-      <c r="J46" s="176"/>
-      <c r="K46" s="176"/>
+      <c r="B46" s="172"/>
+      <c r="C46" s="172"/>
+      <c r="D46" s="172"/>
+      <c r="E46" s="172"/>
+      <c r="F46" s="172"/>
+      <c r="G46" s="172"/>
+      <c r="H46" s="172"/>
+      <c r="I46" s="172"/>
+      <c r="J46" s="172"/>
+      <c r="K46" s="172"/>
     </row>
     <row r="47" spans="1:11" s="65" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="73" t="s">
         <v>121</v>
       </c>
       <c r="B47" s="72"/>
-      <c r="C47" s="177" t="s">
+      <c r="C47" s="173" t="s">
         <v>122</v>
       </c>
-      <c r="D47" s="177"/>
-      <c r="E47" s="177"/>
-      <c r="F47" s="177"/>
-      <c r="G47" s="177"/>
-      <c r="H47" s="177"/>
-      <c r="I47" s="177"/>
-      <c r="J47" s="177"/>
-      <c r="K47" s="177"/>
+      <c r="D47" s="173"/>
+      <c r="E47" s="173"/>
+      <c r="F47" s="173"/>
+      <c r="G47" s="173"/>
+      <c r="H47" s="173"/>
+      <c r="I47" s="173"/>
+      <c r="J47" s="173"/>
+      <c r="K47" s="173"/>
     </row>
     <row r="48" spans="1:11" s="66" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="170"/>
-      <c r="B48" s="170" t="s">
+      <c r="A48" s="176"/>
+      <c r="B48" s="176" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="170" t="s">
+      <c r="C48" s="176" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="170" t="s">
+      <c r="D48" s="176" t="s">
         <v>124</v>
       </c>
-      <c r="E48" s="170" t="s">
+      <c r="E48" s="176" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="170" t="s">
+      <c r="F48" s="176" t="s">
         <v>125</v>
       </c>
-      <c r="G48" s="170" t="s">
+      <c r="G48" s="176" t="s">
         <v>99</v>
       </c>
-      <c r="H48" s="171" t="s">
+      <c r="H48" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="I48" s="172"/>
-      <c r="J48" s="172"/>
-      <c r="K48" s="172"/>
+      <c r="I48" s="184"/>
+      <c r="J48" s="184"/>
+      <c r="K48" s="184"/>
     </row>
     <row r="49" spans="1:11" s="66" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="170"/>
-      <c r="B49" s="170"/>
-      <c r="C49" s="170"/>
-      <c r="D49" s="170"/>
-      <c r="E49" s="170"/>
-      <c r="F49" s="170"/>
-      <c r="G49" s="170"/>
-      <c r="H49" s="178" t="s">
+      <c r="A49" s="176"/>
+      <c r="B49" s="176"/>
+      <c r="C49" s="176"/>
+      <c r="D49" s="176"/>
+      <c r="E49" s="176"/>
+      <c r="F49" s="176"/>
+      <c r="G49" s="176"/>
+      <c r="H49" s="174" t="s">
         <v>127</v>
       </c>
-      <c r="I49" s="179"/>
+      <c r="I49" s="175"/>
       <c r="J49" s="67" t="s">
         <v>128</v>
       </c>
@@ -9460,7 +9450,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="93" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C50" s="68">
         <v>45238</v>
@@ -9478,15 +9468,15 @@
       <c r="G50" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="H50" s="168" t="s">
-        <v>268</v>
-      </c>
-      <c r="I50" s="169"/>
+      <c r="H50" s="181" t="s">
+        <v>264</v>
+      </c>
+      <c r="I50" s="182"/>
       <c r="J50" s="71" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="K50" s="71" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="66" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9494,7 +9484,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="93" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C51" s="68">
         <v>45219</v>
@@ -9512,15 +9502,15 @@
       <c r="G51" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="H51" s="201" t="s">
-        <v>272</v>
-      </c>
-      <c r="I51" s="202"/>
+      <c r="H51" s="185" t="s">
+        <v>268</v>
+      </c>
+      <c r="I51" s="186"/>
       <c r="J51" s="71" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K51" s="71" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="66" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9528,7 +9518,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="93" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C52" s="68">
         <v>45238</v>
@@ -9546,15 +9536,15 @@
       <c r="G52" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="H52" s="201" t="s">
-        <v>272</v>
-      </c>
-      <c r="I52" s="202"/>
+      <c r="H52" s="185" t="s">
+        <v>268</v>
+      </c>
+      <c r="I52" s="186"/>
       <c r="J52" s="71" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K52" s="71" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="66" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9567,6 +9557,15 @@
     <row r="60" spans="1:11" s="66" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:K48"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="A46:K46"/>
@@ -9578,15 +9577,6 @@
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A44:K44"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F52">
     <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
@@ -9637,33 +9627,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="184" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
+      <c r="A1" s="187" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="76"/>
       <c r="B2" s="77"/>
-      <c r="C2" s="164" t="s">
+      <c r="C2" s="165" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="164"/>
+      <c r="D2" s="165"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="81" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -9797,7 +9787,7 @@
     <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>41</v>
       </c>
@@ -9835,9 +9825,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="114" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B2" s="15">
         <v>5</v>
@@ -9873,9 +9863,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="114" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B3" s="15">
         <v>5</v>
@@ -9911,9 +9901,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="114" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B4" s="15">
         <v>6</v>
@@ -9931,9 +9921,9 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="114" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B5" s="15">
         <v>6</v>
@@ -9951,9 +9941,9 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="114" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B6" s="15">
         <v>5</v>
@@ -9971,9 +9961,9 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="114" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B7" s="15">
         <v>2</v>
@@ -9991,7 +9981,7 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -10005,7 +9995,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -10019,7 +10009,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -10033,7 +10023,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -10047,7 +10037,7 @@
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>30</v>
       </c>
@@ -10095,9 +10085,8 @@
         <f>IF(SUM(L2:L11)&gt;0,K12-SUM(L2:L11), "")</f>
         <v/>
       </c>
-      <c r="M12" s="203"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>31</v>
       </c>
@@ -10146,7 +10135,7 @@
         <v>4.4408920985006262E-15</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>63</v>
       </c>
@@ -10195,7 +10184,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>64</v>
       </c>
@@ -10244,7 +10233,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="s">
         <v>67</v>
       </c>
@@ -10274,10 +10263,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10298,119 +10287,119 @@
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="192" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="192"/>
-      <c r="L1" s="192"/>
-      <c r="M1" s="192"/>
-      <c r="N1" s="192"/>
-    </row>
-    <row r="2" spans="1:23" s="95" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="193" t="s">
+    <row r="1" spans="1:14" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="195" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+    </row>
+    <row r="2" spans="1:14" s="95" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="193"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
-      <c r="I2" s="193"/>
-      <c r="J2" s="193"/>
-      <c r="K2" s="193"/>
-      <c r="L2" s="193"/>
-      <c r="M2" s="193"/>
-      <c r="N2" s="193"/>
-    </row>
-    <row r="3" spans="1:23" s="95" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="194" t="s">
+      <c r="B2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="196"/>
+      <c r="G2" s="196"/>
+      <c r="H2" s="196"/>
+      <c r="I2" s="196"/>
+      <c r="J2" s="196"/>
+      <c r="K2" s="196"/>
+      <c r="L2" s="196"/>
+      <c r="M2" s="196"/>
+      <c r="N2" s="196"/>
+    </row>
+    <row r="3" spans="1:14" s="95" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="197" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="197"/>
+    </row>
+    <row r="4" spans="1:14" s="95" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="198" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="198"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="198"/>
+      <c r="N4" s="198"/>
+    </row>
+    <row r="5" spans="1:14" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="199" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="199"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
+      <c r="G5" s="199"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="199"/>
+      <c r="L5" s="199"/>
+      <c r="M5" s="199"/>
+      <c r="N5" s="199"/>
+    </row>
+    <row r="6" spans="1:14" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A7" s="193" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="194"/>
+      <c r="D7" s="193" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="194"/>
+      <c r="G7" s="189" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="189"/>
+      <c r="I7" s="189"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="189"/>
+      <c r="M7" s="193" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="194"/>
-      <c r="H3" s="194"/>
-      <c r="I3" s="194"/>
-      <c r="J3" s="194"/>
-      <c r="K3" s="194"/>
-      <c r="L3" s="194"/>
-      <c r="M3" s="194"/>
-      <c r="N3" s="194"/>
-    </row>
-    <row r="4" spans="1:23" s="95" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="195" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="195"/>
-      <c r="C4" s="195"/>
-      <c r="D4" s="195"/>
-      <c r="E4" s="195"/>
-      <c r="F4" s="195"/>
-      <c r="G4" s="195"/>
-      <c r="H4" s="195"/>
-      <c r="I4" s="195"/>
-      <c r="J4" s="195"/>
-      <c r="K4" s="195"/>
-      <c r="L4" s="195"/>
-      <c r="M4" s="195"/>
-      <c r="N4" s="195"/>
-    </row>
-    <row r="5" spans="1:23" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="196" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="196"/>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
-      <c r="E5" s="196"/>
-      <c r="F5" s="196"/>
-      <c r="G5" s="196"/>
-      <c r="H5" s="196"/>
-      <c r="I5" s="196"/>
-      <c r="J5" s="196"/>
-      <c r="K5" s="196"/>
-      <c r="L5" s="196"/>
-      <c r="M5" s="196"/>
-      <c r="N5" s="196"/>
-    </row>
-    <row r="6" spans="1:23" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A7" s="190" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="191"/>
-      <c r="D7" s="190" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7" s="191"/>
-      <c r="G7" s="186" t="s">
-        <v>136</v>
-      </c>
-      <c r="H7" s="186"/>
-      <c r="I7" s="186"/>
-      <c r="J7" s="186"/>
-      <c r="K7" s="186"/>
-      <c r="M7" s="190" t="s">
-        <v>170</v>
-      </c>
-      <c r="N7" s="191"/>
-    </row>
-    <row r="8" spans="1:23" s="22" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N7" s="194"/>
+    </row>
+    <row r="8" spans="1:14" s="22" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="96" t="s">
         <v>148</v>
       </c>
@@ -10418,7 +10407,7 @@
         <v>138</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E8" s="97" t="s">
         <v>138</v>
@@ -10439,21 +10428,21 @@
         <v>139</v>
       </c>
       <c r="M8" s="97" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="N8" s="97" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
-        <v>149</v>
+        <v>271</v>
       </c>
       <c r="B9" s="98" t="s">
         <v>146</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>153</v>
+        <v>252</v>
       </c>
       <c r="E9" s="98" t="s">
         <v>146</v>
@@ -10475,19 +10464,21 @@
         <v>8</v>
       </c>
       <c r="M9" s="100" t="s">
-        <v>154</v>
-      </c>
-      <c r="N9" s="102"/>
-    </row>
-    <row r="10" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A10" s="94" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="98" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="98"/>
+        <v>151</v>
+      </c>
+      <c r="N9" s="102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A10" s="94"/>
+      <c r="B10" s="98"/>
+      <c r="D10" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10" s="98" t="s">
+        <v>93</v>
+      </c>
       <c r="G10" s="96" t="s">
         <v>137</v>
       </c>
@@ -10499,28 +10490,36 @@
         <v>0</v>
       </c>
       <c r="M10" s="100" t="s">
-        <v>155</v>
-      </c>
-      <c r="N10" s="102"/>
-    </row>
-    <row r="11" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="N10" s="102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="94"/>
       <c r="B11" s="98"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="98"/>
-      <c r="G11" s="186" t="s">
+      <c r="D11" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="189" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="186"/>
-      <c r="I11" s="186"/>
-      <c r="J11" s="186"/>
-      <c r="K11" s="186"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="189"/>
+      <c r="J11" s="189"/>
+      <c r="K11" s="189"/>
       <c r="M11" s="100" t="s">
-        <v>156</v>
-      </c>
-      <c r="N11" s="102"/>
-    </row>
-    <row r="12" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="N11" s="102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="94"/>
       <c r="B12" s="98"/>
       <c r="D12" s="94"/>
@@ -10541,11 +10540,13 @@
         <v>139</v>
       </c>
       <c r="M12" s="100" t="s">
-        <v>179</v>
-      </c>
-      <c r="N12" s="102"/>
-    </row>
-    <row r="13" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="N12" s="102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A13" s="94"/>
       <c r="B13" s="98"/>
       <c r="D13" s="94"/>
@@ -10563,14 +10564,13 @@
         <v>3</v>
       </c>
       <c r="M13" s="100" t="s">
-        <v>157</v>
-      </c>
-      <c r="N13" s="102"/>
-      <c r="W13" s="22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="N13" s="102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A14" s="94"/>
       <c r="B14" s="98"/>
       <c r="D14" s="94"/>
@@ -10586,11 +10586,13 @@
         <v>0</v>
       </c>
       <c r="M14" s="100" t="s">
-        <v>158</v>
-      </c>
-      <c r="N14" s="102"/>
-    </row>
-    <row r="15" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="N14" s="102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A15" s="94"/>
       <c r="B15" s="98"/>
       <c r="D15" s="94"/>
@@ -10608,29 +10610,33 @@
         <v>3</v>
       </c>
       <c r="M15" s="100" t="s">
-        <v>159</v>
-      </c>
-      <c r="N15" s="102"/>
-    </row>
-    <row r="16" spans="1:23" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="N15" s="102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="94"/>
       <c r="B16" s="98"/>
       <c r="D16" s="94"/>
       <c r="E16" s="98"/>
-      <c r="G16" s="187" t="s">
+      <c r="G16" s="190" t="s">
         <v>145</v>
       </c>
-      <c r="H16" s="188"/>
-      <c r="I16" s="188"/>
-      <c r="J16" s="189"/>
+      <c r="H16" s="191"/>
+      <c r="I16" s="191"/>
+      <c r="J16" s="192"/>
       <c r="K16" s="99">
         <f>SUM(K9,K10,K13,K14,K15)</f>
         <v>14</v>
       </c>
       <c r="M16" s="100" t="s">
-        <v>160</v>
-      </c>
-      <c r="N16" s="102"/>
+        <v>157</v>
+      </c>
+      <c r="N16" s="102">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A17" s="94"/>
@@ -10638,9 +10644,11 @@
       <c r="D17" s="94"/>
       <c r="E17" s="98"/>
       <c r="M17" s="100" t="s">
-        <v>161</v>
-      </c>
-      <c r="N17" s="102"/>
+        <v>158</v>
+      </c>
+      <c r="N17" s="102">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A18" s="94"/>
@@ -10648,9 +10656,11 @@
       <c r="D18" s="94"/>
       <c r="E18" s="98"/>
       <c r="M18" s="100" t="s">
-        <v>162</v>
-      </c>
-      <c r="N18" s="102"/>
+        <v>159</v>
+      </c>
+      <c r="N18" s="102">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="94"/>
@@ -10658,9 +10668,11 @@
       <c r="D19" s="94"/>
       <c r="E19" s="98"/>
       <c r="M19" s="100" t="s">
-        <v>163</v>
-      </c>
-      <c r="N19" s="102"/>
+        <v>160</v>
+      </c>
+      <c r="N19" s="102">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A20" s="94"/>
@@ -10668,52 +10680,58 @@
       <c r="D20" s="94"/>
       <c r="E20" s="98"/>
       <c r="M20" s="100" t="s">
-        <v>164</v>
-      </c>
-      <c r="N20" s="102"/>
+        <v>161</v>
+      </c>
+      <c r="N20" s="102">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="M21" s="100" t="s">
-        <v>165</v>
-      </c>
-      <c r="N21" s="102"/>
+        <v>162</v>
+      </c>
+      <c r="N21" s="102">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="M22" s="100" t="s">
-        <v>166</v>
-      </c>
-      <c r="N22" s="102"/>
+        <v>163</v>
+      </c>
+      <c r="N22" s="102">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:14" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="M23" s="101" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N23" s="103">
         <f>SUM(N9:N22)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M24" s="101" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="N24" s="99">
         <f>(N23*0.01)+0.65</f>
-        <v>0.65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M25" s="101" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="N25" s="104">
         <f>K16*N24</f>
-        <v>9.1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M26" s="101" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N26" s="105">
         <v>19</v>
@@ -10721,11 +10739,11 @@
     </row>
     <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="M27" s="106" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N27" s="107">
         <f>N25*N26</f>
-        <v>172.9</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -10761,8 +10779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10784,42 +10802,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="192" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="192"/>
-      <c r="L1" s="192"/>
-      <c r="M1" s="192"/>
-      <c r="N1" s="192"/>
+      <c r="A1" s="195" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="198" t="s">
+      <c r="A3" s="201" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="E3" s="185" t="s">
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
+      <c r="E3" s="188" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="188"/>
+      <c r="K3" s="188"/>
+      <c r="L3" s="188"/>
+      <c r="M3" s="188"/>
+      <c r="N3" s="188"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -10827,61 +10845,61 @@
       </c>
       <c r="B4" s="126">
         <f>'#Estimativa-APF#'!$N$27</f>
-        <v>172.9</v>
+        <v>266</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="199" t="s">
+      <c r="E4" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="197" t="s">
+      <c r="F4" s="200" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197" t="s">
+      <c r="G4" s="200"/>
+      <c r="H4" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197" t="s">
+      <c r="I4" s="200"/>
+      <c r="J4" s="200" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="197"/>
-      <c r="L4" s="197" t="s">
+      <c r="K4" s="200"/>
+      <c r="L4" s="200" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="197"/>
+      <c r="M4" s="200"/>
       <c r="N4" s="112"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="52" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B5" s="26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="199"/>
-      <c r="F5" s="197" t="s">
+      <c r="E5" s="202"/>
+      <c r="F5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197" t="s">
+      <c r="G5" s="200"/>
+      <c r="H5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="197"/>
-      <c r="J5" s="197" t="s">
+      <c r="I5" s="200"/>
+      <c r="J5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="197"/>
-      <c r="L5" s="197" t="s">
+      <c r="K5" s="200"/>
+      <c r="L5" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="197"/>
+      <c r="M5" s="200"/>
       <c r="N5" s="27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -10890,36 +10908,36 @@
       </c>
       <c r="B6" s="127">
         <f>B4+(B4*B5)</f>
-        <v>172.9</v>
+        <v>292.60000000000002</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="199"/>
+      <c r="E6" s="202"/>
       <c r="F6" s="108">
         <f>B6*G6</f>
-        <v>8.6450000000000014</v>
+        <v>14.630000000000003</v>
       </c>
       <c r="G6" s="17">
         <v>0.05</v>
       </c>
       <c r="H6" s="108">
         <f>B4*I6</f>
-        <v>34.580000000000005</v>
+        <v>53.2</v>
       </c>
       <c r="I6" s="17">
         <v>0.2</v>
       </c>
       <c r="J6" s="108">
         <f>B4*K6</f>
-        <v>112.38500000000001</v>
+        <v>172.9</v>
       </c>
       <c r="K6" s="17">
         <v>0.65</v>
       </c>
       <c r="L6" s="108">
         <f>B4*M6</f>
-        <v>17.290000000000003</v>
+        <v>26.6</v>
       </c>
       <c r="M6" s="17">
         <v>0.1</v>
@@ -10931,7 +10949,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="8"/>
       <c r="E7" s="4" t="s">
@@ -10939,35 +10957,35 @@
       </c>
       <c r="F7" s="108">
         <f>F6*G7</f>
-        <v>4.7547500000000014</v>
+        <v>8.0465000000000018</v>
       </c>
       <c r="G7" s="17">
         <v>0.55000000000000004</v>
       </c>
       <c r="H7" s="108">
         <f>H6*I7</f>
-        <v>10.374000000000001</v>
+        <v>15.96</v>
       </c>
       <c r="I7" s="17">
         <v>0.3</v>
       </c>
       <c r="J7" s="108">
         <f>J6*K7</f>
-        <v>13.4862</v>
+        <v>20.748000000000001</v>
       </c>
       <c r="K7" s="17">
         <v>0.12</v>
       </c>
       <c r="L7" s="108">
         <f>L6*M7</f>
-        <v>0.86450000000000016</v>
+        <v>1.33</v>
       </c>
       <c r="M7" s="17">
         <v>0.05</v>
       </c>
       <c r="N7" s="111">
         <f>SUM(F7,H7,J7,L7)</f>
-        <v>29.47945</v>
+        <v>46.084500000000006</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -10975,7 +10993,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="15">
-        <v>40</v>
+        <v>12.5</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>29</v>
@@ -10985,35 +11003,35 @@
       </c>
       <c r="F8" s="108">
         <f>F6*G8</f>
-        <v>1.2967500000000001</v>
+        <v>2.1945000000000001</v>
       </c>
       <c r="G8" s="17">
         <v>0.15</v>
       </c>
       <c r="H8" s="108">
         <f>H6*I8</f>
-        <v>6.9160000000000013</v>
+        <v>10.64</v>
       </c>
       <c r="I8" s="17">
         <v>0.2</v>
       </c>
       <c r="J8" s="108">
         <f>J6*K8</f>
-        <v>11.238500000000002</v>
+        <v>17.290000000000003</v>
       </c>
       <c r="K8" s="17">
         <v>0.1</v>
       </c>
       <c r="L8" s="108">
         <f>L6*M8</f>
-        <v>0.86450000000000016</v>
+        <v>1.33</v>
       </c>
       <c r="M8" s="17">
         <v>0.05</v>
       </c>
       <c r="N8" s="111">
         <f t="shared" ref="N8:N14" si="0">SUM(F8,H8,J8,L8)</f>
-        <v>20.315750000000001</v>
+        <v>31.454500000000003</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -11031,35 +11049,35 @@
       </c>
       <c r="F9" s="108">
         <f>F6*G9</f>
-        <v>0.17290000000000003</v>
+        <v>0.29260000000000008</v>
       </c>
       <c r="G9" s="17">
         <v>0.02</v>
       </c>
       <c r="H9" s="108">
         <f>H6*I9</f>
-        <v>6.9160000000000013</v>
+        <v>10.64</v>
       </c>
       <c r="I9" s="17">
         <v>0.2</v>
       </c>
       <c r="J9" s="108">
         <f>J6*K9</f>
-        <v>44.954000000000008</v>
+        <v>69.160000000000011</v>
       </c>
       <c r="K9" s="17">
         <v>0.4</v>
       </c>
       <c r="L9" s="108">
         <f>L6*M9</f>
-        <v>2.5935000000000001</v>
+        <v>3.99</v>
       </c>
       <c r="M9" s="17">
         <v>0.15</v>
       </c>
       <c r="N9" s="111">
         <f t="shared" si="0"/>
-        <v>54.636400000000009</v>
+        <v>84.082599999999999</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -11068,7 +11086,7 @@
       </c>
       <c r="B10" s="11">
         <f>(B7*B8)*B9</f>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>13</v>
@@ -11078,35 +11096,35 @@
       </c>
       <c r="F10" s="108">
         <f>F6*G10</f>
-        <v>0.43225000000000008</v>
+        <v>0.73150000000000015</v>
       </c>
       <c r="G10" s="17">
         <v>0.05</v>
       </c>
       <c r="H10" s="108">
         <f>H6*I10</f>
-        <v>2.7664000000000004</v>
+        <v>4.2560000000000002</v>
       </c>
       <c r="I10" s="17">
         <v>0.08</v>
       </c>
       <c r="J10" s="108">
         <f>J6*K10</f>
-        <v>11.238500000000002</v>
+        <v>17.290000000000003</v>
       </c>
       <c r="K10" s="17">
         <v>0.1</v>
       </c>
       <c r="L10" s="108">
         <f>L6*M10</f>
-        <v>1.7290000000000003</v>
+        <v>2.66</v>
       </c>
       <c r="M10" s="17">
         <v>0.1</v>
       </c>
       <c r="N10" s="111">
         <f t="shared" si="0"/>
-        <v>16.166150000000002</v>
+        <v>24.937500000000004</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -11115,7 +11133,7 @@
       </c>
       <c r="B11" s="43">
         <f>B6/B10*2</f>
-        <v>4.3224999999999998</v>
+        <v>7.8026666666666671</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>28</v>
@@ -11132,28 +11150,28 @@
       </c>
       <c r="H11" s="108">
         <f>H6*I11</f>
-        <v>0.6916000000000001</v>
+        <v>1.0640000000000001</v>
       </c>
       <c r="I11" s="17">
         <v>0.02</v>
       </c>
       <c r="J11" s="108">
         <f>J6*K11</f>
-        <v>5.619250000000001</v>
+        <v>8.6450000000000014</v>
       </c>
       <c r="K11" s="17">
         <v>0.05</v>
       </c>
       <c r="L11" s="108">
         <f>L6*M11</f>
-        <v>1.7290000000000003</v>
+        <v>2.66</v>
       </c>
       <c r="M11" s="17">
         <v>0.1</v>
       </c>
       <c r="N11" s="111">
         <f t="shared" si="0"/>
-        <v>8.0398500000000013</v>
+        <v>12.369000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -11162,7 +11180,7 @@
       </c>
       <c r="B12" s="43">
         <f>B11/4</f>
-        <v>1.0806249999999999</v>
+        <v>1.9506666666666668</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>51</v>
@@ -11172,7 +11190,7 @@
       </c>
       <c r="F12" s="109">
         <f>SUM(F7:F11)</f>
-        <v>6.6566500000000017</v>
+        <v>11.265100000000002</v>
       </c>
       <c r="G12" s="50">
         <f t="shared" ref="G12:M12" si="1">SUM(G7:G11)</f>
@@ -11180,7 +11198,7 @@
       </c>
       <c r="H12" s="109">
         <f t="shared" si="1"/>
-        <v>27.664000000000005</v>
+        <v>42.56</v>
       </c>
       <c r="I12" s="50">
         <f t="shared" si="1"/>
@@ -11188,7 +11206,7 @@
       </c>
       <c r="J12" s="109">
         <f t="shared" si="1"/>
-        <v>86.536450000000002</v>
+        <v>133.13300000000001</v>
       </c>
       <c r="K12" s="50">
         <f t="shared" si="1"/>
@@ -11196,7 +11214,7 @@
       </c>
       <c r="L12" s="109">
         <f t="shared" si="1"/>
-        <v>7.7805000000000009</v>
+        <v>11.97</v>
       </c>
       <c r="M12" s="50">
         <f t="shared" si="1"/>
@@ -11206,11 +11224,11 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B13" s="48">
         <f>B11/B9</f>
-        <v>2.1612499999999999</v>
+        <v>3.9013333333333335</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>49</v>
@@ -11220,35 +11238,35 @@
       </c>
       <c r="F13" s="108">
         <f>F6*G13</f>
-        <v>0.25935000000000002</v>
+        <v>0.43890000000000007</v>
       </c>
       <c r="G13" s="17">
         <v>0.03</v>
       </c>
       <c r="H13" s="108">
         <f>H6*I13</f>
-        <v>2.7664000000000004</v>
+        <v>4.2560000000000002</v>
       </c>
       <c r="I13" s="17">
         <v>0.08</v>
       </c>
       <c r="J13" s="108">
         <f>J6*K13</f>
-        <v>14.610050000000001</v>
+        <v>22.477</v>
       </c>
       <c r="K13" s="17">
         <v>0.13</v>
       </c>
       <c r="L13" s="108">
         <f>L6*M13</f>
-        <v>5.1870000000000003</v>
+        <v>7.98</v>
       </c>
       <c r="M13" s="17">
         <v>0.3</v>
       </c>
       <c r="N13" s="111">
         <f t="shared" si="0"/>
-        <v>22.822800000000004</v>
+        <v>35.151899999999998</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -11257,35 +11275,35 @@
       </c>
       <c r="F14" s="108">
         <f>F6*G14</f>
-        <v>1.7290000000000003</v>
+        <v>2.9260000000000006</v>
       </c>
       <c r="G14" s="17">
         <v>0.2</v>
       </c>
       <c r="H14" s="108">
         <f>H6*I14</f>
-        <v>4.1496000000000004</v>
+        <v>6.3840000000000003</v>
       </c>
       <c r="I14" s="17">
         <v>0.12</v>
       </c>
       <c r="J14" s="108">
         <f>J6*K14</f>
-        <v>11.238500000000002</v>
+        <v>17.290000000000003</v>
       </c>
       <c r="K14" s="17">
         <v>0.1</v>
       </c>
       <c r="L14" s="108">
         <f>L6*M14</f>
-        <v>4.3225000000000007</v>
+        <v>6.65</v>
       </c>
       <c r="M14" s="17">
         <v>0.25</v>
       </c>
       <c r="N14" s="111">
         <f t="shared" si="0"/>
-        <v>21.439600000000002</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -11294,7 +11312,7 @@
       </c>
       <c r="F15" s="109">
         <f>SUM(F13:F14)</f>
-        <v>1.9883500000000003</v>
+        <v>3.3649000000000004</v>
       </c>
       <c r="G15" s="50">
         <f t="shared" ref="G15:M15" si="2">SUM(G13:G14)</f>
@@ -11302,7 +11320,7 @@
       </c>
       <c r="H15" s="109">
         <f t="shared" si="2"/>
-        <v>6.9160000000000004</v>
+        <v>10.64</v>
       </c>
       <c r="I15" s="50">
         <f t="shared" si="2"/>
@@ -11310,7 +11328,7 @@
       </c>
       <c r="J15" s="109">
         <f t="shared" si="2"/>
-        <v>25.848550000000003</v>
+        <v>39.767000000000003</v>
       </c>
       <c r="K15" s="50">
         <f t="shared" si="2"/>
@@ -11318,7 +11336,7 @@
       </c>
       <c r="L15" s="109">
         <f t="shared" si="2"/>
-        <v>9.509500000000001</v>
+        <v>14.63</v>
       </c>
       <c r="M15" s="50">
         <f t="shared" si="2"/>
@@ -11327,17 +11345,17 @@
       <c r="N15" s="49"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="198" t="s">
+      <c r="A16" s="201" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="198"/>
-      <c r="C16" s="198"/>
+      <c r="B16" s="201"/>
+      <c r="C16" s="201"/>
       <c r="E16" s="27" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F16" s="110">
         <f>F12+F15</f>
-        <v>8.6450000000000014</v>
+        <v>14.630000000000003</v>
       </c>
       <c r="G16" s="28">
         <f t="shared" ref="G16:M16" si="3">G12+G15</f>
@@ -11345,7 +11363,7 @@
       </c>
       <c r="H16" s="110">
         <f t="shared" si="3"/>
-        <v>34.580000000000005</v>
+        <v>53.2</v>
       </c>
       <c r="I16" s="28">
         <f t="shared" si="3"/>
@@ -11353,7 +11371,7 @@
       </c>
       <c r="J16" s="110">
         <f t="shared" si="3"/>
-        <v>112.38500000000001</v>
+        <v>172.9</v>
       </c>
       <c r="K16" s="28">
         <f t="shared" si="3"/>
@@ -11361,7 +11379,7 @@
       </c>
       <c r="L16" s="110">
         <f t="shared" si="3"/>
-        <v>17.290000000000003</v>
+        <v>26.6</v>
       </c>
       <c r="M16" s="28">
         <f t="shared" si="3"/>
@@ -11369,7 +11387,7 @@
       </c>
       <c r="N16" s="113">
         <f>SUM(N7:N11,N13,N14)</f>
-        <v>172.90000000000003</v>
+        <v>267.33</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -11388,7 +11406,7 @@
       </c>
       <c r="B18" s="5">
         <f>B6*B17</f>
-        <v>3458</v>
+        <v>5852</v>
       </c>
       <c r="C18" s="2"/>
       <c r="L18" s="1"/>
@@ -11399,7 +11417,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C19" s="2"/>
       <c r="N19" s="1"/>
@@ -11410,7 +11428,7 @@
       </c>
       <c r="B20" s="6">
         <f>B18*B19</f>
-        <v>0</v>
+        <v>585.20000000000005</v>
       </c>
       <c r="C20" s="2"/>
       <c r="L20" s="1"/>
@@ -11422,7 +11440,7 @@
       </c>
       <c r="B21" s="25">
         <f>B18+B20</f>
-        <v>3458</v>
+        <v>6437.2</v>
       </c>
       <c r="C21" s="2"/>
       <c r="N21" s="1"/>
@@ -11443,7 +11461,7 @@
       </c>
       <c r="B23" s="7">
         <f>B21*B22</f>
-        <v>691.6</v>
+        <v>1287.44</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -11453,7 +11471,7 @@
       </c>
       <c r="B24" s="25">
         <f>B21+B23</f>
-        <v>4149.6000000000004</v>
+        <v>7724.6399999999994</v>
       </c>
       <c r="C24" s="2"/>
     </row>

</xml_diff>